<commit_message>
dialogue system with choice; player unlocked
</commit_message>
<xml_diff>
--- a/data/dialogues.xlsx
+++ b/data/dialogues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Godot\4.4.1\Projects\palettelock\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86C4ADB-7478-47B5-8130-690F631DE338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C668FB-A1B3-40F7-9658-880A2B928F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{12C1E853-8D79-44E1-86E5-BDEAA7F657E5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t>MARIANNE</t>
   </si>
@@ -69,9 +69,6 @@
     <t>CHOICE</t>
   </si>
   <si>
-    <t>I knew it was at huzz</t>
-  </si>
-  <si>
     <t>IT WAS AT PLUZZ?</t>
   </si>
   <si>
@@ -94,6 +91,27 @@
   </si>
   <si>
     <t>tell me[huzz,pluzz,gruzz]</t>
+  </si>
+  <si>
+    <t>JEFF_HUZZ</t>
+  </si>
+  <si>
+    <t>GOTO</t>
+  </si>
+  <si>
+    <t>But what's your name?[GRINGO,MORTIMER,GIBBY]</t>
+  </si>
+  <si>
+    <t>your name is gringo?</t>
+  </si>
+  <si>
+    <t>I knew your mortimer?</t>
+  </si>
+  <si>
+    <t>bitch ass gibby</t>
+  </si>
+  <si>
+    <t>I forgot your name</t>
   </si>
 </sst>
 </file>
@@ -457,11 +475,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9628B97A-2D30-47EA-9687-081196DB5F56}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,19 +491,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -590,7 +608,7 @@
         <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -598,10 +616,10 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -612,7 +630,13 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -620,13 +644,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -634,7 +652,13 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -642,21 +666,90 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14</v>
       </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
       <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>